<commit_message>
working on project structure (planning stage)
</commit_message>
<xml_diff>
--- a/planning/userstories_creaturecomforts.xlsx
+++ b/planning/userstories_creaturecomforts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_FullStack\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF6B8F3-6AE8-420A-BA33-268FF345AD4A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281AB309-3D72-4206-80ED-97B0377DE2D2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{11BBF541-E308-4458-A585-171A38B365F5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="3" xr2:uid="{11BBF541-E308-4458-A585-171A38B365F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
   <si>
     <t>Project 5</t>
   </si>
@@ -247,9 +247,6 @@
     <t>PRODUCTS</t>
   </si>
   <si>
-    <t>COMMUNITY</t>
-  </si>
-  <si>
     <t>USER</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
     <t>threads and comments under products</t>
   </si>
   <si>
-    <t>blog</t>
-  </si>
-  <si>
     <t>tags</t>
   </si>
   <si>
@@ -410,6 +404,9 @@
   </si>
   <si>
     <t>A website that allows a user to add product to a wishlist or 'like' it for future reference.</t>
+  </si>
+  <si>
+    <t>COMMUNITY/BLOG</t>
   </si>
 </sst>
 </file>
@@ -595,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -655,6 +652,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1313,14 +1312,14 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.85546875" bestFit="1" customWidth="1"/>
@@ -1350,14 +1349,14 @@
       <c r="B2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="16" t="s">
+      <c r="G2" s="26" t="s">
         <v>72</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1368,16 +1367,13 @@
         <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
         <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1388,16 +1384,13 @@
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1408,23 +1401,20 @@
         <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" t="s">
         <v>84</v>
-      </c>
-      <c r="G6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1435,10 +1425,10 @@
         <v>38</v>
       </c>
       <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" t="s">
         <v>85</v>
-      </c>
-      <c r="G7" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1448,8 +1438,11 @@
       <c r="B8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D8" t="s">
-        <v>88</v>
+      <c r="D8" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1459,9 +1452,6 @@
       <c r="B9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -1470,6 +1460,11 @@
       <c r="B10" s="11" t="s">
         <v>50</v>
       </c>
+      <c r="D10" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -1478,6 +1473,9 @@
       <c r="B11" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="D11" s="26" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
@@ -1499,7 +1497,7 @@
         <v>47</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -1518,16 +1516,16 @@
         <v>52</v>
       </c>
       <c r="E15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" t="s">
         <v>117</v>
-      </c>
-      <c r="F15" t="s">
-        <v>119</v>
       </c>
       <c r="H15" t="s">
         <v>60</v>
       </c>
       <c r="I15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1538,26 +1536,26 @@
         <v>38</v>
       </c>
       <c r="D16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" t="s">
         <v>116</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>118</v>
       </c>
-      <c r="F16" t="s">
-        <v>120</v>
-      </c>
       <c r="H16" t="s">
+        <v>119</v>
+      </c>
+      <c r="I16" t="s">
         <v>121</v>
-      </c>
-      <c r="I16" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="I17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1602,6 +1600,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1612,8 +1611,8 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,127 +1622,127 @@
         <v>70</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1755,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA748F1-FE2A-4EF9-9AD5-1D4503484BA6}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1818,12 +1817,12 @@
     </row>
     <row r="7" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
temp styling changes to test correct wiring of static files
</commit_message>
<xml_diff>
--- a/planning/userstories_creaturecomforts.xlsx
+++ b/planning/userstories_creaturecomforts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_FullStack\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281AB309-3D72-4206-80ED-97B0377DE2D2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E60520-3A5F-46A6-B22D-E68E7F4CD232}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="3" xr2:uid="{11BBF541-E308-4458-A585-171A38B365F5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{11BBF541-E308-4458-A585-171A38B365F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="129">
   <si>
     <t>Project 5</t>
   </si>
@@ -407,6 +407,15 @@
   </si>
   <si>
     <t>COMMUNITY/BLOG</t>
+  </si>
+  <si>
+    <t>action to perform + persona = benefit from it</t>
+  </si>
+  <si>
+    <t>As a potential buyer, I would like to see the list of all products and their prices, so I could decide which one I like best</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
 </sst>
 </file>
@@ -515,7 +524,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,8 +555,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -588,11 +603,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -646,14 +726,28 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1025,7 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F811C58F-B57F-4564-81E4-C786B6BD75A6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
@@ -1038,267 +1132,299 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8DC7F8-A7B3-4BA4-8D49-16D8CE5053D3}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="11" customWidth="1"/>
     <col min="2" max="2" width="73.28515625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="29.7109375" style="11"/>
+    <col min="3" max="3" width="46" style="32" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="29.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="36" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="36" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="20" customFormat="1" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="20" customFormat="1" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="E2" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="E3" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="E4" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="E5" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="E6" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="E7" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:4" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="31"/>
+    </row>
+    <row r="9" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="E9" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="E11" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="E12" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:4" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="E15" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="30"/>
+      <c r="D17" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="E17" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="E18" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:4" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="31"/>
+    </row>
+    <row r="20" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="E20" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="E21" s="21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="E22" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="30"/>
+      <c r="D23" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="E23" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="30"/>
+      <c r="D24" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="E24" s="21" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1312,7 +1438,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="K21" sqref="K21:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,13 +1475,13 @@
       <c r="B2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1438,10 +1564,10 @@
       <c r="B8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1460,7 +1586,7 @@
       <c r="B10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="25" t="s">
         <v>87</v>
       </c>
       <c r="E10" s="16"/>
@@ -1473,7 +1599,7 @@
       <c r="B11" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="25" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1609,88 +1735,91 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="27" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>70</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -1784,7 +1913,7 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="8" t="s">

</xml_diff>

<commit_message>
temp styling changes to ensure correct wiring of static files
</commit_message>
<xml_diff>
--- a/planning/userstories_creaturecomforts.xlsx
+++ b/planning/userstories_creaturecomforts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_FullStack\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281AB309-3D72-4206-80ED-97B0377DE2D2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E60520-3A5F-46A6-B22D-E68E7F4CD232}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="3" xr2:uid="{11BBF541-E308-4458-A585-171A38B365F5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{11BBF541-E308-4458-A585-171A38B365F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="129">
   <si>
     <t>Project 5</t>
   </si>
@@ -407,6 +407,15 @@
   </si>
   <si>
     <t>COMMUNITY/BLOG</t>
+  </si>
+  <si>
+    <t>action to perform + persona = benefit from it</t>
+  </si>
+  <si>
+    <t>As a potential buyer, I would like to see the list of all products and their prices, so I could decide which one I like best</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
 </sst>
 </file>
@@ -515,7 +524,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,8 +555,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -588,11 +603,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFE2E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -646,14 +726,28 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1025,7 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F811C58F-B57F-4564-81E4-C786B6BD75A6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
@@ -1038,267 +1132,299 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8DC7F8-A7B3-4BA4-8D49-16D8CE5053D3}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="11" customWidth="1"/>
     <col min="2" max="2" width="73.28515625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="29.7109375" style="11"/>
+    <col min="3" max="3" width="46" style="32" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="29.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="36" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="36" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="20" customFormat="1" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="20" customFormat="1" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="E2" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="E3" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="E4" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="E5" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="E6" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="E7" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:4" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="31"/>
+    </row>
+    <row r="9" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="E9" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="E11" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="E12" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:4" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="E15" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="30"/>
+      <c r="D17" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="E17" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="E18" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:4" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="31"/>
+    </row>
+    <row r="20" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="E20" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="E21" s="21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="E22" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="30"/>
+      <c r="D23" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="E23" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="30"/>
+      <c r="D24" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="E24" s="21" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1312,7 +1438,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="K21" sqref="K21:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,13 +1475,13 @@
       <c r="B2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1438,10 +1564,10 @@
       <c r="B8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1460,7 +1586,7 @@
       <c r="B10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="25" t="s">
         <v>87</v>
       </c>
       <c r="E10" s="16"/>
@@ -1473,7 +1599,7 @@
       <c r="B11" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="25" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1609,88 +1735,91 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="27" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>70</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -1784,7 +1913,7 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="8" t="s">

</xml_diff>

<commit_message>
I updated the index view and added the chartjs javascript.
I also maintained the User Story document guiding the creation of the website.
</commit_message>
<xml_diff>
--- a/planning/userstories_creaturecomforts.xlsx
+++ b/planning/userstories_creaturecomforts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_FullStack\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E60520-3A5F-46A6-B22D-E68E7F4CD232}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34797C76-6EBF-4780-B3C0-BCB0E6D28013}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{11BBF541-E308-4458-A585-171A38B365F5}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="135">
   <si>
     <t>Project 5</t>
   </si>
@@ -415,14 +415,32 @@
     <t>As a potential buyer, I would like to see the list of all products and their prices, so I could decide which one I like best</t>
   </si>
   <si>
-    <t>example</t>
+    <t>As a potential buyer, XYZ wants to see the list of all products and their prices, so she can  decide which one she likes best.</t>
+  </si>
+  <si>
+    <t>As a potential buyer, XYZ wants to have access to the opinions of previous customers, soshe can make an informed decision.</t>
+  </si>
+  <si>
+    <t>OVERALL</t>
+  </si>
+  <si>
+    <t>"" XYZ wants to be able to access his/her own data, so he/she can track her preferences.</t>
+  </si>
+  <si>
+    <t>As a site member, XYZ can view the profiles of other members so that she can find others she might want to connect with</t>
+  </si>
+  <si>
+    <t>As a site visitor, XYZ can send his comments via a contact, so he can get in touch with the webmaster</t>
+  </si>
+  <si>
+    <t>As a site visitor,XYZ has an advanced search option that lets him/her fill in a form of search criteria (country, state, trainer name, date range, word in description, etc.) so he/she can quickly find whathe/she is looking for</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +538,19 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF596161"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -649,12 +680,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FFDFE2E5"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFDFE2E5"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -664,8 +691,12 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color rgb="FFDFE2E5"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -737,17 +768,21 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,14 +1170,14 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="11" customWidth="1"/>
     <col min="2" max="2" width="73.28515625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="46" style="32" customWidth="1"/>
+    <col min="3" max="3" width="46" style="30" customWidth="1"/>
     <col min="4" max="4" width="41.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.28515625" style="11" customWidth="1"/>
     <col min="6" max="16384" width="29.7109375" style="11"/>
@@ -1155,21 +1190,21 @@
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>128</v>
+      <c r="C1" s="31" t="s">
+        <v>130</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="20" customFormat="1" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="20" customFormat="1" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="32" t="s">
         <v>127</v>
       </c>
       <c r="D2" s="27" t="s">
@@ -1179,14 +1214,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="21" customFormat="1" ht="44.25" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="30"/>
+      <c r="C3" s="28" t="s">
+        <v>128</v>
+      </c>
       <c r="D3" s="21" t="s">
         <v>58</v>
       </c>
@@ -1194,11 +1231,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="21" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="28" t="s">
+        <v>129</v>
+      </c>
       <c r="D4" s="21" t="s">
         <v>64</v>
       </c>
@@ -1206,11 +1245,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="21" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="28" t="s">
+        <v>131</v>
+      </c>
       <c r="D5" s="21" t="s">
         <v>53</v>
       </c>
@@ -1218,11 +1259,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="21" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="28" t="s">
+        <v>132</v>
+      </c>
       <c r="D6" s="21" t="s">
         <v>53</v>
       </c>
@@ -1230,11 +1273,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="21" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="30" t="s">
+        <v>133</v>
+      </c>
       <c r="D7" s="21" t="s">
         <v>54</v>
       </c>
@@ -1243,16 +1288,18 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="31"/>
-    </row>
-    <row r="9" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="C8" s="29"/>
+    </row>
+    <row r="9" spans="1:5" s="21" customFormat="1" ht="72.75" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="28" t="s">
+        <v>134</v>
+      </c>
       <c r="D9" s="21" t="s">
         <v>53</v>
       </c>
@@ -1264,7 +1311,7 @@
       <c r="B10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="30"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="21" t="s">
         <v>63</v>
       </c>
@@ -1276,7 +1323,7 @@
       <c r="B11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="21" t="s">
         <v>55</v>
       </c>
@@ -1288,7 +1335,7 @@
       <c r="B12" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="21" t="s">
         <v>56</v>
       </c>
@@ -1300,7 +1347,7 @@
       <c r="B13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="21" t="s">
         <v>57</v>
       </c>
@@ -1309,7 +1356,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="31"/>
+      <c r="C14" s="29"/>
     </row>
     <row r="15" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
@@ -1318,7 +1365,7 @@
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="21" t="s">
         <v>59</v>
       </c>
@@ -1330,7 +1377,6 @@
       <c r="B16" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="30"/>
       <c r="D16" s="21" t="s">
         <v>60</v>
       </c>
@@ -1342,7 +1388,7 @@
       <c r="B17" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="21" t="s">
         <v>61</v>
       </c>
@@ -1354,7 +1400,7 @@
       <c r="B18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="30"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="21" t="s">
         <v>62</v>
       </c>
@@ -1363,7 +1409,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="31"/>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
@@ -1372,7 +1418,7 @@
       <c r="B20" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="30"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="21" t="s">
         <v>65</v>
       </c>
@@ -1384,7 +1430,7 @@
       <c r="B21" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="30"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="21" t="s">
         <v>66</v>
       </c>
@@ -1396,7 +1442,7 @@
       <c r="B22" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="30"/>
+      <c r="C22" s="28"/>
       <c r="D22" s="21" t="s">
         <v>67</v>
       </c>
@@ -1408,7 +1454,7 @@
       <c r="B23" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="30"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="21" t="s">
         <v>68</v>
       </c>
@@ -1420,7 +1466,7 @@
       <c r="B24" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="30"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="21" t="s">
         <v>69</v>
       </c>
@@ -1430,6 +1476,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
I updated the readme.md an testing.md files.
I am preparing to submit this project to be reviewed.
</commit_message>
<xml_diff>
--- a/planning/userstories_creaturecomforts.xlsx
+++ b/planning/userstories_creaturecomforts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_FullStack\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34797C76-6EBF-4780-B3C0-BCB0E6D28013}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD13102-1D58-4473-B9B4-D94B3656D5EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{11BBF541-E308-4458-A585-171A38B365F5}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="150">
   <si>
     <t>Project 5</t>
   </si>
@@ -37,12 +37,6 @@
     <t>CREATURE COMFORT</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Purpose of visit</t>
-  </si>
-  <si>
     <t>Concept</t>
   </si>
   <si>
@@ -52,63 +46,18 @@
     <t>Camille</t>
   </si>
   <si>
-    <t>Camille wants to share nice things with friends and family members.</t>
-  </si>
-  <si>
-    <t>Camille wants to treat herself.</t>
-  </si>
-  <si>
     <t>Harry</t>
   </si>
   <si>
-    <t>Camille wants a tailored-made shopping experience</t>
-  </si>
-  <si>
-    <t>Harry wants to spoil his wife on special occasions.</t>
-  </si>
-  <si>
-    <t>Harry wants an easy way to offer presents to members of his family.</t>
-  </si>
-  <si>
-    <t>Harry is on the mend due to an injury and wants to recover comfortably.</t>
-  </si>
-  <si>
     <t>Mike</t>
   </si>
   <si>
-    <t>Mike follows trends and wants to test the suscription box concept.</t>
-  </si>
-  <si>
-    <t>Mike is busy and wants a quick way to gather the items he needs.</t>
-  </si>
-  <si>
-    <t>Mike wants to try new things and discover items based on his preferences.</t>
-  </si>
-  <si>
     <t>Lou</t>
   </si>
   <si>
-    <t>Lou wants to spend quality time with his wife and daughters.</t>
-  </si>
-  <si>
-    <t>Lou is busy and does not like to shop or spend too much time online.</t>
-  </si>
-  <si>
-    <t>Lou believes in quality over quantity when purchasing items.</t>
-  </si>
-  <si>
-    <t>Lou is interested by items that everyone in his household can benefit from.</t>
-  </si>
-  <si>
     <t>How the website responds to those wants</t>
   </si>
   <si>
-    <t>Mike does not want to pay a lot to get items.</t>
-  </si>
-  <si>
-    <t>Harry wants value for his money.</t>
-  </si>
-  <si>
     <t>What the user wants from the service offered</t>
   </si>
   <si>
@@ -121,18 +70,6 @@
     <t>INCONVENIENTS</t>
   </si>
   <si>
-    <t>Camille wants to get variety and discover new things.</t>
-  </si>
-  <si>
-    <t>Camille wants to share her finds and good ideas.</t>
-  </si>
-  <si>
-    <t>Harry wants to learn and find ideas that he benefit from at home.</t>
-  </si>
-  <si>
-    <t>Lou is curious to see what other parents do with their kids in their down time.</t>
-  </si>
-  <si>
     <t>recurring payments from your customers</t>
   </si>
   <si>
@@ -412,35 +349,143 @@
     <t>action to perform + persona = benefit from it</t>
   </si>
   <si>
-    <t>As a potential buyer, I would like to see the list of all products and their prices, so I could decide which one I like best</t>
-  </si>
-  <si>
-    <t>As a potential buyer, XYZ wants to see the list of all products and their prices, so she can  decide which one she likes best.</t>
-  </si>
-  <si>
-    <t>As a potential buyer, XYZ wants to have access to the opinions of previous customers, soshe can make an informed decision.</t>
-  </si>
-  <si>
-    <t>OVERALL</t>
-  </si>
-  <si>
-    <t>"" XYZ wants to be able to access his/her own data, so he/she can track her preferences.</t>
-  </si>
-  <si>
-    <t>As a site member, XYZ can view the profiles of other members so that she can find others she might want to connect with</t>
-  </si>
-  <si>
-    <t>As a site visitor, XYZ can send his comments via a contact, so he can get in touch with the webmaster</t>
-  </si>
-  <si>
-    <t>As a site visitor,XYZ has an advanced search option that lets him/her fill in a form of search criteria (country, state, trainer name, date range, word in description, etc.) so he/she can quickly find whathe/she is looking for</t>
+    <t>As a [persona]</t>
+  </si>
+  <si>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>so she can interact with other people online with the same interests.</t>
+  </si>
+  <si>
+    <t>wants to access information easily</t>
+  </si>
+  <si>
+    <t>so he does not have to remember a password or username.</t>
+  </si>
+  <si>
+    <t>so he can afford all features and recommend them to his friends.</t>
+  </si>
+  <si>
+    <t>so he can return to it more easily.</t>
+  </si>
+  <si>
+    <t>so she can decide which item or option she likes best</t>
+  </si>
+  <si>
+    <t>wants to see what previous customers think of their purchase</t>
+  </si>
+  <si>
+    <t>to find what he really wants to purchase.</t>
+  </si>
+  <si>
+    <t>wants to visit the website's products by using categories or a search function</t>
+  </si>
+  <si>
+    <t>wants to include his family's need in his shopping</t>
+  </si>
+  <si>
+    <t>so he can spend quality time with them.</t>
+  </si>
+  <si>
+    <t>because Lou does not like to shop or spend too much time online.</t>
+  </si>
+  <si>
+    <t>so he can come up with new activities on a budget.</t>
+  </si>
+  <si>
+    <t>so he can have a personalised browsing experience.</t>
+  </si>
+  <si>
+    <t>wants to send her comments and feedback easily</t>
+  </si>
+  <si>
+    <t>so she can get in touch with the webmaster if there is a problem with her browsing experience.</t>
+  </si>
+  <si>
+    <t>as it is the most convenient device in his house for browsing.</t>
+  </si>
+  <si>
+    <t>since she always accesses websites on the go.</t>
+  </si>
+  <si>
+    <t>wants to use her smartphone to go on the internet and visit Creature Comforts</t>
+  </si>
+  <si>
+    <t>wants to try the trendiest boxes of Creature Comforts</t>
+  </si>
+  <si>
+    <t>wants to be able to access the Creature Comforts' website on his iMac</t>
+  </si>
+  <si>
+    <t>so he can shop online using his computer at home.</t>
+  </si>
+  <si>
+    <t>wants to view the profiles of other members on Creature Comforts' blog</t>
+  </si>
+  <si>
+    <t>so that he can find others he might want to connect with.</t>
+  </si>
+  <si>
+    <t>wants to access Creature Comforts' website using his iPad</t>
+  </si>
+  <si>
+    <t>wants to see on the Creature Comforts' blog what other parents do with their kids in their down time</t>
+  </si>
+  <si>
+    <t>wants to encourage small business and business ventures like creature Comforts</t>
+  </si>
+  <si>
+    <t>because he believes in buying local and trusting personable companies.</t>
+  </si>
+  <si>
+    <t>wants to use a nickname on Creature Comforts' blog</t>
+  </si>
+  <si>
+    <t>so he can retrieve and update his login details during future visits.</t>
+  </si>
+  <si>
+    <t>wants to have a reset password option when he registers on Creature Comforts</t>
+  </si>
+  <si>
+    <t>wants to track information he likes on the blog</t>
+  </si>
+  <si>
+    <t>wants to browse the content of a website without having to pay a premium</t>
+  </si>
+  <si>
+    <t>wants to send messages to the webmaster without leaving Creature Comforts' website</t>
+  </si>
+  <si>
+    <t>so he does not forget to send the message and remembers what he wants to say.</t>
+  </si>
+  <si>
+    <t>wants to browse Creature Comforts' website without having to log in</t>
+  </si>
+  <si>
+    <t>so she can decide which one she wants to buy.</t>
+  </si>
+  <si>
+    <t>wants to see the list of all products in CC's shop, their prices and frequency</t>
+  </si>
+  <si>
+    <t>so that I can [realize a reward]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want to [do something] </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,12 +587,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF24292E"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -555,7 +594,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -592,8 +631,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -684,26 +729,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFDFE2E5"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -730,7 +760,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -745,43 +774,67 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1167,312 +1220,375 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8DC7F8-A7B3-4BA4-8D49-16D8CE5053D3}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="29.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="73.28515625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="46" style="30" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.28515625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="29.7109375" style="11"/>
+    <col min="1" max="1" width="25" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" style="28" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" style="28" hidden="1" customWidth="1"/>
+    <col min="6" max="16384" width="29.7109375" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:5" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="31" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="20" customFormat="1" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="27" t="s">
+      <c r="C13" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="21" customFormat="1" ht="44.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+    </row>
+    <row r="16" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="21" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="21" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="21" t="s">
+      <c r="B16" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
+      <c r="B18" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+    </row>
+    <row r="19" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="21" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="21" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="29"/>
-    </row>
-    <row r="9" spans="1:5" s="21" customFormat="1" ht="72.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="28" t="s">
+      <c r="B21" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="21" t="s">
+      <c r="C22" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
+      <c r="B23" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="32" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="29"/>
-    </row>
-    <row r="15" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="29"/>
-    </row>
-    <row r="20" spans="1:5" s="21" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>50</v>
-      </c>
+      <c r="E24" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
+      <c r="B25" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="C26" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1499,276 +1615,276 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="G5" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="B13" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="B15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="I15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="D6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="B16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="I17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" t="s">
-        <v>115</v>
-      </c>
-      <c r="F15" t="s">
-        <v>117</v>
-      </c>
-      <c r="H15" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>114</v>
-      </c>
-      <c r="E16" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H16" t="s">
-        <v>119</v>
-      </c>
-      <c r="I16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="I17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>50</v>
+      <c r="B22" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1791,134 +1907,134 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="17" t="s">
-        <v>91</v>
-      </c>
       <c r="R1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>96</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>90</v>
+      <c r="A6" s="16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>103</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1938,67 +2054,67 @@
   <cols>
     <col min="1" max="1" width="53.140625" style="9" customWidth="1"/>
     <col min="2" max="3" width="30" style="8"/>
-    <col min="4" max="4" width="30" style="14"/>
+    <col min="4" max="4" width="30" style="13"/>
     <col min="5" max="16384" width="30" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>110</v>
+      <c r="A7" s="17" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>111</v>
+      <c r="A8" s="17" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>